<commit_message>
remake builtin data with new format
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/canada/canada.xlsx
+++ b/inst/extdata/projects/canada/canada.xlsx
@@ -7,11 +7,12 @@
   </bookViews>
   <sheets>
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Site status" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Site feasibility" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Feature data" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Expectation of “Maintain”" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Expectation of “Restore”" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Feasibility data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Feature data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Expectation of “Maintain”" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Expectation of “Restore”" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Expectation of “Signage”" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="metadata" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -22,7 +23,7 @@
     <author>X</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,6 +47,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Add signs to informing of local catch quotas</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -78,7 +91,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Ecologically important land and coastline in Nova Scotia</t>
+          <t xml:space="preserve">Ecologically important coastal area</t>
         </r>
       </text>
     </comment>
@@ -128,6 +141,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Add signs to informing of local catch quotas</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -160,7 +185,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Ecologically important land and coastline in Nova Scotia</t>
+          <t xml:space="preserve">Ecologically important coastal area</t>
         </r>
       </text>
     </comment>
@@ -186,30 +211,6 @@
     <author>X</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Maintenance actions</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Restoration actions to improve ecological integrity</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -218,7 +219,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Pond in Nova Scotia</t>
+          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
         </r>
       </text>
     </comment>
@@ -230,7 +231,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Bay in Nova Scotia</t>
+          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
         </r>
       </text>
     </comment>
@@ -242,19 +243,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Ecologically important land and coastline in Nova Scotia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Bay community in the Canadian province of Nova Scotia</t>
+          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
         </r>
       </text>
     </comment>
@@ -268,6 +257,42 @@
     <author>X</author>
   </authors>
   <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -276,7 +301,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone that is regularly flooded by the tides</t>
+          <t xml:space="preserve">Pond in Nova Scotia</t>
         </r>
       </text>
     </comment>
@@ -288,7 +313,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plant species</t>
+          <t xml:space="preserve">Bay in Nova Scotia</t>
         </r>
       </text>
     </comment>
@@ -300,7 +325,19 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains fresh water, and is frequently flooded</t>
+          <t xml:space="preserve">Ecologically important coastal area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Bay community in the Canadian province of Nova Scotia</t>
         </r>
       </text>
     </comment>
@@ -322,7 +359,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone that is regularly flooded by the tides</t>
+          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
         </r>
       </text>
     </comment>
@@ -334,7 +371,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plant species</t>
+          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
         </r>
       </text>
     </comment>
@@ -346,7 +383,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains fresh water, and is frequently flooded</t>
+          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
         </r>
       </text>
     </comment>
@@ -382,7 +419,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Ecologically important land and coastline in Nova Scotia</t>
+          <t xml:space="preserve">Ecologically important coastal area</t>
         </r>
       </text>
     </comment>
@@ -416,7 +453,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone that is regularly flooded by the tides</t>
+          <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
         </r>
       </text>
     </comment>
@@ -428,7 +465,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plant species</t>
+          <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
         </r>
       </text>
     </comment>
@@ -440,7 +477,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains fresh water, and is frequently flooded</t>
+          <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
         </r>
       </text>
     </comment>
@@ -476,7 +513,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Ecologically important land and coastline in Nova Scotia</t>
+          <t xml:space="preserve">Ecologically important coastal area</t>
         </r>
       </text>
     </comment>
@@ -497,7 +534,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
@@ -514,12 +551,18 @@
     <t xml:space="preserve">Latitude (DD)</t>
   </si>
   <si>
+    <t xml:space="preserve">Current status</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cost of “Maintain”</t>
   </si>
   <si>
     <t xml:space="preserve">Cost of “Restore”</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of “Signage”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Johnston's Pond</t>
   </si>
   <si>
@@ -535,18 +578,6 @@
     <t xml:space="preserve">Round Bay</t>
   </si>
   <si>
-    <t xml:space="preserve">Please enter status information for your sites into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are currently being implemented within each site. By default, none of the actions are currently implemented within each site. To specify that a certain a certain action can be implemented within a certain site, please enter value of “1”. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “Maintain”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “Restore”</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
   </si>
   <si>
@@ -559,6 +590,9 @@
     <t xml:space="preserve">Feasibility of “Restore”</t>
   </si>
   <si>
+    <t xml:space="preserve">Feasibility of “Signage”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
   </si>
   <si>
@@ -602,6 +636,69 @@
   </si>
   <si>
     <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Restore” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter information for your “Signage” action into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Signage” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pond in Nova Scotia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay in Nova Scotia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restoration actions to improve ecological integrity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecologically important coastal area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add signs to informing of local catch quotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay community in the Canadian province of Nova Scotia</t>
   </si>
 </sst>
 </file>
@@ -805,50 +902,54 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:E7" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:E7"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:G7" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:G7"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Longitude (DD)"/>
     <tableColumn id="3" name="Latitude (DD)"/>
-    <tableColumn id="4" name="Cost of “Maintain”"/>
-    <tableColumn id="5" name="Cost of “Restore”"/>
+    <tableColumn id="4" name="Current status"/>
+    <tableColumn id="5" name="Cost of “Maintain”"/>
+    <tableColumn id="6" name="Cost of “Restore”"/>
+    <tableColumn id="7" name="Cost of “Signage”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:C7" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:C7"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:D7" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:D7"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Site ID"/>
-    <tableColumn id="2" name="Status of “Maintain”"/>
-    <tableColumn id="3" name="Status of “Restore”"/>
+    <tableColumn id="2" name="Feasibility of “Maintain”"/>
+    <tableColumn id="3" name="Feasibility of “Restore”"/>
+    <tableColumn id="4" name="Feasibility of “Signage”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C7" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:C7"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Site ID"/>
-    <tableColumn id="2" name="Feasibility of “Maintain”"/>
-    <tableColumn id="3" name="Feasibility of “Restore”"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C6" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C6" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Target threshold amount"/>
     <tableColumn id="3" name="Relative importance (weight)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:D7" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:D7"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Site ID"/>
+    <tableColumn id="2" name="Amount of “Salt Marsh”"/>
+    <tableColumn id="3" name="Amount of “ACPF”"/>
+    <tableColumn id="4" name="Amount of “Freshwater Wetland”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -875,6 +976,21 @@
     <tableColumn id="2" name="Amount of “Salt Marsh”"/>
     <tableColumn id="3" name="Amount of “ACPF”"/>
     <tableColumn id="4" name="Amount of “Freshwater Wetland”"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:F5" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="site_ids"/>
+    <tableColumn id="2" name="action_ids"/>
+    <tableColumn id="3" name="feature_ids"/>
+    <tableColumn id="4" name="site_descriptions"/>
+    <tableColumn id="5" name="action_descriptions"/>
+    <tableColumn id="6" name="feature_descriptions"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1168,10 +1284,12 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="24.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="28.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="27.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="27.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="26.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="24.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="28.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="27.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="27.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1182,6 +1300,8 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" ht="120" customHeight="1">
       <c r="A2" s="2"/>
@@ -1191,6 +1311,8 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -1208,58 +1330,80 @@
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>-64.9857460961314</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>43.7602324948388</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>-65.9081692527981</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>43.7654869380519</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>-64.9080895986714</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>43.8180985398522</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>-65.3498991696735</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>43.5805904606311</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -1276,7 +1420,7 @@
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="D4:E7">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="E4:G7">
       <formula1>0</formula1>
       <formula2>1e+06</formula2>
     </dataValidation>
@@ -1287,125 +1431,22 @@
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'meta'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="30.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="29.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="30.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="30.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="20" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" ht="100" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B4:C7">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>B4=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>B4=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:C7">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <legacyDrawing r:id="rIdvml"/>
-  <tableParts count="1">
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1418,38 +1459,43 @@
     <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="35.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="34.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="35.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="34.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="35.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>1</v>
@@ -1457,10 +1503,13 @@
       <c r="C4" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>1</v>
@@ -1468,10 +1517,13 @@
       <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="D5" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>1</v>
@@ -1479,15 +1531,21 @@
       <c r="C6" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="D6" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1497,7 +1555,7 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:C7">
+  <conditionalFormatting sqref="B4:D7">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>B4=0</formula>
     </cfRule>
@@ -1506,7 +1564,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:C7">
+    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:D7">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1515,12 +1573,12 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1538,59 +1596,59 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1613,6 +1671,106 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="32.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="26.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="40.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="40.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" ht="160" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:D7">
+      <formula1>0</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
+  <tableParts count="1">
     <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
@@ -1638,7 +1796,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1646,7 +1804,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1656,18 +1814,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1675,7 +1833,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1683,7 +1841,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1691,7 +1849,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1738,7 +1896,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1746,7 +1904,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1756,18 +1914,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1775,7 +1933,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1783,7 +1941,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1791,7 +1949,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1816,4 +1974,122 @@
     <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create builtin data with values
</commit_message>
<xml_diff>
--- a/inst/extdata/projects/canada/canada.xlsx
+++ b/inst/extdata/projects/canada/canada.xlsx
@@ -566,136 +566,136 @@
     <t xml:space="preserve">Johnston's Pond</t>
   </si>
   <si>
+    <t xml:space="preserve">Restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lobster Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Joli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “Maintain”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “Restore”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “Signage”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target threshold amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative importance (weight)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salt Marsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freshwater Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter information for your “Maintain” action into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Maintain” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of “Salt Marsh”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of “ACPF”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of “Freshwater Wetland”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter information for your “Restore” action into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Restore” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter information for your “Signage” action into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Signage” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pond in Nova Scotia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay in Nova Scotia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restoration actions to improve ecological integrity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecologically important coastal area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add signs to informing of local catch quotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Lobster Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Joli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feasibility of “Maintain”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feasibility of “Restore”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feasibility of “Signage”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light gray cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feature ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target threshold amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative importance (weight)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salt Marsh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freshwater Wetland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter information for your “Maintain” action into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Maintain” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount of “Salt Marsh”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount of “ACPF”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount of “Freshwater Wetland”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter information for your “Restore” action into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Restore” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter information for your “Signage” action into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “Signage” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">action_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feature_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site_descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">action_descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feature_descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pond in Nova Scotia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintenance actions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal ecosystem in the upper coastal intertidal zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bay in Nova Scotia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restoration actions to improve ecological integrity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlantic Coastal Plain Flora are a group of 94 herbaceous plants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecologically important coastal area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add signs to informing of local catch quotas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-tidal, non-forested marsh wetland that contains freshwater, and is frequently flooded</t>
   </si>
   <si>
     <t xml:space="preserve">Bay community in the Canadian province of Nova Scotia</t>
@@ -1350,9 +1350,15 @@
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="E4" s="5" t="n">
+        <v>172</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>308</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>575</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -1365,15 +1371,21 @@
         <v>43.7654869380519</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>115</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>255</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>477</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>-64.9080895986714</v>
@@ -1382,15 +1394,21 @@
         <v>43.8180985398522</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>196</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>277</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>562</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>-65.3498991696735</v>
@@ -1401,9 +1419,15 @@
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="5" t="n">
+        <v>188</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>316</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>561</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -1422,7 +1446,7 @@
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="E4:G7">
       <formula1>0</formula1>
-      <formula2>1e+06</formula2>
+      <formula2>1000000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,7 +1490,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1474,7 +1498,7 @@
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1484,13 +1508,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -1523,7 +1547,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>1</v>
@@ -1537,7 +1561,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>1</v>
@@ -1596,59 +1620,59 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1684,7 @@
   <dataValidations count="2">
     <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B6">
       <formula1>0</formula1>
-      <formula2>1e+06</formula2>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C6">
       <formula1>0</formula1>
@@ -1696,7 +1720,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1704,7 +1728,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1714,46 +1738,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -1796,7 +1844,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1804,7 +1852,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1814,46 +1862,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>99</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -1896,7 +1968,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1904,7 +1976,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1914,46 +1986,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>91</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>77</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -1986,22 +2082,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -2009,10 +2105,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -2029,59 +2125,59 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>